<commit_message>
Adjunto: - Mejoras en la explicación de restriciones y sugerencias - Restricciones y sugerencias: Documento de req. - Restricciones y sugerencias: Casos de uso y mejorado: Diagramas de caso de uso: general y un nivel de explotacion - Restricciones y sugerencias: Análisis del sistema FALTA EXPLICACION DE NUEVAS TABLAS - Diagrama del modelo contextual mejorado - Documento de prototipos mejorado: con diagrama de navegación para cada modulo: FALTAN NUEVOS PANTALLAZOS
</commit_message>
<xml_diff>
--- a/documentacion/Documentacion_final/Tareas especificas de la documentacion.xlsx
+++ b/documentacion/Documentacion_final/Tareas especificas de la documentacion.xlsx
@@ -16,23 +16,49 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>tareas</t>
-  </si>
-  <si>
-    <t>cambiar el nombre de clinico por el de usuario</t>
-  </si>
-  <si>
-    <t>palabras clave en todos los documentos</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t>FALTA</t>
+  </si>
+  <si>
+    <t>DOCUMENTO</t>
+  </si>
+  <si>
+    <t>DESCRIPCION</t>
+  </si>
+  <si>
+    <t>Documento de requisitos</t>
+  </si>
+  <si>
+    <t>pantallazos de toda la parte servidora</t>
+  </si>
+  <si>
+    <t>Documento de plan de proyecto</t>
+  </si>
+  <si>
+    <t>IP servidor de desarrollo</t>
+  </si>
+  <si>
+    <t>analisis del sistema</t>
+  </si>
+  <si>
+    <t>Explicacion de las tablas que faltan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -60,8 +86,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -363,27 +390,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>